<commit_message>
Cleaned, imputed, standardized, bootstrapped data update
Bootsrapped data too big - on google drive
</commit_message>
<xml_diff>
--- a/data/FinalVars.xlsx
+++ b/data/FinalVars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuyuchen/Documents/GitHub/ENAR-Risk-Factors-Analyses/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011F0C1D-967C-8E44-8BCA-DAA2ECD43B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB5A8F0-3A94-4540-B52A-59A9267096F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33660" yWindow="3440" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{02CB9FAE-DCD3-B84F-90F8-ABD8C174A7D0}"/>
+    <workbookView xWindow="4080" yWindow="500" windowWidth="30240" windowHeight="17980" xr2:uid="{02CB9FAE-DCD3-B84F-90F8-ABD8C174A7D0}"/>
   </bookViews>
   <sheets>
     <sheet name="QuesVars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="224">
   <si>
     <t>ACD011A - Speak English at home - NHW or NHB</t>
   </si>
@@ -699,6 +699,18 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>BPQ020 - Ever told you had high blood pressure</t>
+  </si>
+  <si>
+    <t>BPQ040A - Taking prescription for hypertension</t>
+  </si>
+  <si>
+    <t>BPQ150 - Taking high blood pressure medication</t>
+  </si>
+  <si>
+    <t>BPQ050A - Now taking prescribed medicine for HBP</t>
   </si>
 </sst>
 </file>
@@ -1103,10 +1115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35511AA6-1791-594B-B856-993C898D471A}">
-  <dimension ref="A1:A76"/>
+  <dimension ref="A1:A80"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1489,6 +1501,26 @@
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -4786,7 +4818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B51116-9844-4742-95FD-8D92C7ABAD1C}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+    <sheetView topLeftCell="A50" workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update cleaned data - remove duplicate dummy vars
</commit_message>
<xml_diff>
--- a/data/FinalVars.xlsx
+++ b/data/FinalVars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuyuchen/Documents/GitHub/ENAR-Risk-Factors-Analyses/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB5A8F0-3A94-4540-B52A-59A9267096F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA06F5C-4507-6F4B-90A4-C0427A3C4B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="500" windowWidth="30240" windowHeight="17980" xr2:uid="{02CB9FAE-DCD3-B84F-90F8-ABD8C174A7D0}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17980" activeTab="3" xr2:uid="{02CB9FAE-DCD3-B84F-90F8-ABD8C174A7D0}"/>
   </bookViews>
   <sheets>
     <sheet name="QuesVars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="222">
   <si>
     <t>ACD011A - Speak English at home - NHW or NHB</t>
   </si>
@@ -309,12 +309,6 @@
   </si>
   <si>
     <t>OCQ660 - Hours per day exposed to very loud noise</t>
-  </si>
-  <si>
-    <t>OHQ030 - When did you last visit a dentist</t>
-  </si>
-  <si>
-    <t>OHQ033 - Main reason for last dental visit</t>
   </si>
   <si>
     <t>OHQ845 - Rate the health of your teeth and gums</t>
@@ -1115,22 +1109,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35511AA6-1791-594B-B856-993C898D471A}">
-  <dimension ref="A1:A80"/>
+  <dimension ref="A1:A78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
@@ -1479,12 +1473,12 @@
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="A72" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="A73" s="1" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1494,13 +1488,13 @@
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>109</v>
+      <c r="A75" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>110</v>
+      <c r="A76" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
@@ -1511,16 +1505,6 @@
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -1540,12 +1524,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
@@ -1750,147 +1734,147 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
@@ -4818,355 +4802,355 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B51116-9844-4742-95FD-8D92C7ABAD1C}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D69">
         <f>+D65</f>
@@ -5175,72 +5159,72 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Code and Data and Feature after repull the data
</commit_message>
<xml_diff>
--- a/data/FinalVars.xlsx
+++ b/data/FinalVars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuyuchen/Documents/GitHub/ENAR-Risk-Factors-Analyses/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA06F5C-4507-6F4B-90A4-C0427A3C4B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D725EE-C298-ED40-90C3-578FDADDBC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17980" activeTab="3" xr2:uid="{02CB9FAE-DCD3-B84F-90F8-ABD8C174A7D0}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17980" xr2:uid="{02CB9FAE-DCD3-B84F-90F8-ABD8C174A7D0}"/>
   </bookViews>
   <sheets>
     <sheet name="QuesVars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="223">
   <si>
     <t>ACD011A - Speak English at home - NHW or NHB</t>
   </si>
@@ -705,6 +705,9 @@
   </si>
   <si>
     <t>BPQ050A - Now taking prescribed medicine for HBP</t>
+  </si>
+  <si>
+    <t>ALQ130 - Avg # alcohol drinks/day - past 12 mos</t>
   </si>
 </sst>
 </file>
@@ -1109,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35511AA6-1791-594B-B856-993C898D471A}">
-  <dimension ref="A1:A78"/>
+  <dimension ref="A1:A79"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1284,226 +1287,231 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>221</v>
       </c>
     </row>
@@ -4802,7 +4810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B51116-9844-4742-95FD-8D92C7ABAD1C}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>

</xml_diff>